<commit_message>
Added filepath to LCIA Implementation
</commit_message>
<xml_diff>
--- a/ExcelTool_GeneratorInput_Template.xlsx
+++ b/ExcelTool_GeneratorInput_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF74D2DF-D0AC-4091-8309-CE858CF467E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0366464-396E-4727-8EB2-EDB1AEDD7388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -1009,7 +1009,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1421" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="441">
   <si>
     <t>input</t>
   </si>
@@ -2597,6 +2597,12 @@
   </si>
   <si>
     <t>3.7.1</t>
+  </si>
+  <si>
+    <t>LCIA implementation file path</t>
+  </si>
+  <si>
+    <t>C:\Users\SarahSchmidt\Desktop\Databases\ecoinvent\LCIA Implementation v3.8.xlsx</t>
   </si>
 </sst>
 </file>
@@ -5660,10 +5666,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDD7C88C-20AB-446E-9AA2-8B598F1EB83E}">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5839,6 +5845,14 @@
       </c>
       <c r="B28" s="4" t="s">
         <v>438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="13" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>439</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -9997,7 +10011,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -10012,7 +10026,7 @@
     <col min="8" max="16384" width="9.08984375" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
revised compost yields (stylized case study on biowaste management)
</commit_message>
<xml_diff>
--- a/ExcelTool_GeneratorInput_Template.xlsx
+++ b/ExcelTool_GeneratorInput_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9ECA83E-6B71-4C8F-BA3F-7746B86534F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64EA69C-AE4F-44BE-9FAA-30408F3CCD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -5670,7 +5670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A3D566-44A5-479B-A2A9-A44ABD46E4C9}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -7058,8 +7058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J112"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H89" sqref="H89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.90625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -7070,7 +7070,8 @@
     <col min="6" max="6" width="42.90625" style="1"/>
     <col min="7" max="7" width="16.90625" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="42.90625" style="1"/>
   </cols>
   <sheetData>
@@ -7939,7 +7940,7 @@
         <v>10</v>
       </c>
       <c r="H29" s="64">
-        <v>-0.8</v>
+        <v>-0.35</v>
       </c>
       <c r="I29" s="65" t="s">
         <v>12</v>
@@ -8389,7 +8390,7 @@
         <v>10</v>
       </c>
       <c r="H44" s="66">
-        <v>-0.9</v>
+        <v>-0.45</v>
       </c>
       <c r="I44" s="68" t="s">
         <v>12</v>
@@ -9259,7 +9260,7 @@
         <v>10</v>
       </c>
       <c r="H73" s="64">
-        <v>-0.8</v>
+        <v>-0.35</v>
       </c>
       <c r="I73" s="65" t="s">
         <v>12</v>
@@ -9709,7 +9710,7 @@
         <v>10</v>
       </c>
       <c r="H88" s="66">
-        <v>-0.9</v>
+        <v>-0.45</v>
       </c>
       <c r="I88" s="68" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
added predefined parameters (case study: biowaste management)
</commit_message>
<xml_diff>
--- a/ExcelTool_GeneratorInput_Template.xlsx
+++ b/ExcelTool_GeneratorInput_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahSchmidt\Documents\sourcetree\MoEWe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64EA69C-AE4F-44BE-9FAA-30408F3CCD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BED4F8-504A-49FA-8EE1-78B26CC08774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -1006,7 +1006,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="474">
   <si>
     <t>input</t>
   </si>
@@ -2799,6 +2799,45 @@
   </si>
   <si>
     <t>EWU-Component "Environmental value of discarded materials" calculated per weighting method.</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>share of biowaste to home composting</t>
+  </si>
+  <si>
+    <t>industrial biowaste treatment: share to anaerobic digestion</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>industrial biowaste treatment: transport to treatment facilities</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>-P2</t>
+  </si>
+  <si>
+    <t>-1+P2</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>-1+P3</t>
+  </si>
+  <si>
+    <t>-P3</t>
   </si>
 </sst>
 </file>
@@ -3123,7 +3162,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -3198,12 +3237,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3410,6 +3473,28 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="12" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="17" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -6315,7 +6400,7 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7059,7 +7144,7 @@
   <dimension ref="A1:J112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="42.90625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -7165,7 +7250,9 @@
       <c r="I3" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="50"/>
+      <c r="J3" s="101" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
@@ -7195,7 +7282,9 @@
       <c r="I4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="50"/>
+      <c r="J4" s="101" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="51" t="s">
@@ -7555,7 +7644,9 @@
       <c r="I16" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="60"/>
+      <c r="J16" s="102" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="59" t="s">
@@ -7585,7 +7676,9 @@
       <c r="I17" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="J17" s="60"/>
+      <c r="J17" s="102" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="59" t="s">
@@ -7645,7 +7738,9 @@
       <c r="I19" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="60"/>
+      <c r="J19" s="60" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="61" t="s">
@@ -7705,7 +7800,9 @@
       <c r="I21" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J21" s="62"/>
+      <c r="J21" s="103" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="61" t="s">
@@ -7735,7 +7832,9 @@
       <c r="I22" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="62"/>
+      <c r="J22" s="103" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="61" t="s">
@@ -7795,7 +7894,9 @@
       <c r="I24" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="J24" s="62"/>
+      <c r="J24" s="62" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="63" t="s">
@@ -10445,31 +10546,87 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E40A9123-B5A2-440C-9957-36B1335A3358}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" style="95" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" style="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" style="95" customWidth="1"/>
+    <col min="4" max="4" width="15" style="95" customWidth="1"/>
+    <col min="5" max="16384" width="10.90625" style="95"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
+      <c r="A1" s="96" t="s">
         <v>440</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="96" t="s">
         <v>439</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="96" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>441</v>
+      <c r="E1" s="94" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="97" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2" s="97" t="s">
+        <v>463</v>
+      </c>
+      <c r="C2" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="99" t="s">
+        <v>467</v>
+      </c>
+      <c r="E2" s="97" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A3" s="97" t="s">
+        <v>465</v>
+      </c>
+      <c r="B3" s="98" t="s">
+        <v>464</v>
+      </c>
+      <c r="C3" s="100">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="99" t="s">
+        <v>467</v>
+      </c>
+      <c r="E3" s="97" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25" x14ac:dyDescent="0.25">
+      <c r="A4" s="97" t="s">
+        <v>471</v>
+      </c>
+      <c r="B4" s="98" t="s">
+        <v>466</v>
+      </c>
+      <c r="C4" s="97">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="97" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="97" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>